<commit_message>
Ahead with the TSR. Most of the user interface done #4
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Technical Service Report</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Repair:</t>
-  </si>
-  <si>
-    <t>A-asd-asd-asd</t>
   </si>
   <si>
     <t>Issue description:</t>
@@ -414,6 +411,69 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -423,93 +483,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,32 +510,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,15 +633,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>501650</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>88900</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -700,15 +697,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>501650</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>88900</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -764,15 +761,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>501650</xdr:colOff>
+          <xdr:colOff>504825</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>88900</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1115,41 +1112,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1160,7 +1157,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1170,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1184,7 +1181,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1194,14 +1191,14 @@
       <c r="E10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1212,7 +1209,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -1222,12 +1219,12 @@
       <c r="E12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -1235,42 +1232,42 @@
       <c r="C14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="39" t="s">
+      <c r="E14" s="67"/>
+      <c r="F14" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41" t="s">
+      <c r="G14" s="67"/>
+      <c r="H14" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="40"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="27"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="27"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I14" s="67"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1278,235 +1275,233 @@
       <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="42"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="41"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="25"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="54"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="27"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="27"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="27"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
+      <c r="B26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="C26" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="27"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="27"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="27"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="30"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="27"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="30"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="27"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="30"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="29"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="42"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="46"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="48"/>
+      <c r="C35" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="25"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A35" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="55" t="s">
+      <c r="H35" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="63" t="s">
+      <c r="I35" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="57"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="62"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A37" s="54"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="49"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14">
@@ -1514,13 +1509,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A38" s="26"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="27"/>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="29"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18">
@@ -1528,13 +1523,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="27"/>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="18">
@@ -1542,13 +1537,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="27"/>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="30"/>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" s="18">
@@ -1556,13 +1551,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="27"/>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="30"/>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" s="18">
@@ -1570,13 +1565,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A42" s="28"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="29"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
       <c r="I42" s="19">
@@ -1584,13 +1579,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C43" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="69"/>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="34"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
       <c r="I43" s="22">
@@ -1598,58 +1593,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C44" s="67" t="s">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="69"/>
-      <c r="I44" s="22"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C45" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="69"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="34"/>
       <c r="I45" s="22">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C46" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="68"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="69"/>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="34"/>
       <c r="I46" s="22"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C47" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="64">
+    <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C47" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="23">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="65"/>
-      <c r="I47" s="66"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="H47" s="24"/>
+      <c r="I47" s="25"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1666,42 +1697,6 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1717,15 +1712,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>501650</xdr:colOff>
+                    <xdr:colOff>504825</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>88900</xdr:colOff>
+                    <xdr:colOff>85725</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>104775</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1739,15 +1734,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>501650</xdr:colOff>
+                    <xdr:colOff>504825</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>88900</xdr:colOff>
+                    <xdr:colOff>85725</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>104775</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1761,15 +1756,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>7</xdr:col>
-                    <xdr:colOff>501650</xdr:colOff>
+                    <xdr:colOff>504825</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>88900</xdr:colOff>
+                    <xdr:colOff>85725</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>104775</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
Python script implemented in order to print the tsr worksheet in PDF (using LabView was too complicated). Close #5
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Initiate TSR done (excel ranges). Started with populateTSR #2
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -37,12 +37,6 @@
     <t>City:</t>
   </si>
   <si>
-    <t>Country:</t>
-  </si>
-  <si>
-    <t>Ref:</t>
-  </si>
-  <si>
     <t>Contact:</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
   <si>
     <t>SubTotal
 (AUD)</t>
-  </si>
-  <si>
-    <t>Labour Cost</t>
   </si>
   <si>
     <t>Shipping</t>
@@ -138,6 +129,15 @@
   </si>
   <si>
     <t>Discount (AUD)</t>
+  </si>
+  <si>
+    <t>Post Code:</t>
+  </si>
+  <si>
+    <t>Country:</t>
+  </si>
+  <si>
+    <t>Labour Hour</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -393,12 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,6 +405,137 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,31 +545,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,109 +563,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1112,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I44" sqref="A44:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,21 +1135,21 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1158,7 +1163,7 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
@@ -1182,19 +1187,19 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="11" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="3" t="s">
-        <v>7</v>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="I10" s="7"/>
     </row>
@@ -1210,477 +1215,443 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>8</v>
+      <c r="A12" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
+      <c r="E12" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="E14" s="42"/>
+      <c r="F14" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="67"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="30"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="75">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="30"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="72"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="42"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="31"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="56"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="44" t="s">
+      <c r="B26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="45"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="29"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="29"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="29"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="31"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="58"/>
+      <c r="C35" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="30"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="30"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="30"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="30"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="30"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="30"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="30"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="30"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="42"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="46"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="48"/>
-      <c r="C35" s="47" t="s">
+      <c r="H35" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="55" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14">
+      <c r="A37" s="56"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12">
         <f>H37*G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18">
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16">
         <f t="shared" ref="I38:I43" si="0">H38*G38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18">
+      <c r="A41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19">
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22">
+      <c r="C43" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="70"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
-      <c r="I44" s="22"/>
+      <c r="C44" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="71"/>
+      <c r="I44" s="20"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="34"/>
-      <c r="I45" s="22">
+      <c r="C45" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="71"/>
+      <c r="I45" s="20">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
-      <c r="I46" s="22"/>
+      <c r="C46" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="71"/>
+      <c r="I46" s="20"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="23">
+      <c r="C47" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="66">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="24"/>
-      <c r="I47" s="25"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="68"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
+  <mergeCells count="53">
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1697,6 +1668,43 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Graphic interface done. Still some issues in populating the excel file #4
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -434,12 +434,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,7 +461,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -563,8 +566,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="A44:I44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,24 +1159,26 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1190,14 +1219,14 @@
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="24" t="s">
         <v>31</v>
       </c>
@@ -1224,9 +1253,9 @@
       <c r="E12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,30 +1266,30 @@
       <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="41" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="43"/>
+      <c r="H14" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
-      <c r="C15" s="75">
+      <c r="C15" s="32">
         <v>0.41666666666666669</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="34"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1271,7 +1300,7 @@
       <c r="E16" s="29"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="34"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1282,10 +1311,10 @@
       <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="3"/>
@@ -1294,23 +1323,23 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
-      <c r="C18" s="32"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="28"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="31"/>
       <c r="C19" s="33"/>
       <c r="D19" s="30"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="31"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1329,37 +1358,37 @@
       <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
+      <c r="A22" s="76"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="78"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="29"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="81"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="29"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="81"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
@@ -1369,10 +1398,10 @@
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="29"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="81"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
@@ -1381,81 +1410,81 @@
       <c r="B26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="29"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="81"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="29"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="81"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="29"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="81"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="29"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="81"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="29"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="81"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="29"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="81"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="31"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="84"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
@@ -1471,44 +1500,44 @@
       <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="57" t="s">
+      <c r="B35" s="59"/>
+      <c r="C35" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="63" t="s">
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="65" t="s">
+      <c r="H35" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="65" t="s">
+      <c r="I35" s="66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12">
@@ -1520,8 +1549,8 @@
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="28"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
       <c r="F38" s="29"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
@@ -1534,8 +1563,8 @@
       <c r="A39" s="28"/>
       <c r="B39" s="29"/>
       <c r="C39" s="28"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
       <c r="F39" s="29"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
@@ -1548,8 +1577,8 @@
       <c r="A40" s="28"/>
       <c r="B40" s="29"/>
       <c r="C40" s="28"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="29"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
@@ -1562,8 +1591,8 @@
       <c r="A41" s="28"/>
       <c r="B41" s="29"/>
       <c r="C41" s="28"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
       <c r="F41" s="29"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
@@ -1576,8 +1605,8 @@
       <c r="A42" s="30"/>
       <c r="B42" s="31"/>
       <c r="C42" s="30"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
       <c r="F42" s="31"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
@@ -1587,12 +1616,12 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="72"/>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="20">
@@ -1601,49 +1630,49 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="72"/>
       <c r="I44" s="20"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="72"/>
       <c r="I45" s="20">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="69" t="s">
+      <c r="C46" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="72"/>
       <c r="I46" s="20"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="72" t="s">
+      <c r="C47" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="66">
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="67">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="67"/>
-      <c r="I47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="69"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">

</xml_diff>

<commit_message>
Added start/end hours in TSR #7. Graphic interface for TSR finished #4
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -413,6 +413,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -422,96 +485,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,32 +512,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -592,6 +565,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,7 +1145,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,21 +1164,21 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1219,14 +1219,14 @@
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="24" t="s">
         <v>31</v>
       </c>
@@ -1253,9 +1253,9 @@
       <c r="E12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1266,42 +1266,40 @@
       <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="42" t="s">
+      <c r="E14" s="78"/>
+      <c r="F14" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44" t="s">
+      <c r="G14" s="78"/>
+      <c r="H14" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="78"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="32">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="29"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="29"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1311,97 +1309,97 @@
       <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="84"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="42"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="31"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="44"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="25" t="s">
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="78"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="69"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="80"/>
-      <c r="I23" s="81"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="72"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="82"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="81"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="72"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="81"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="72"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
@@ -1410,134 +1408,134 @@
       <c r="B26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="81"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="72"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="81"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="72"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="81"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="72"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
-      <c r="I29" s="81"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="72"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="81"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="80"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="81"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="84"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="75"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="27"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="58" t="s">
+      <c r="B35" s="50"/>
+      <c r="C35" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="64" t="s">
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="66" t="s">
+      <c r="H35" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="66" t="s">
+      <c r="I35" s="57" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="60"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="57"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12">
@@ -1546,12 +1544,12 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="29"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="32"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
       <c r="I38" s="16">
@@ -1560,12 +1558,12 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="29"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
       <c r="I39" s="16">
@@ -1574,12 +1572,12 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="29"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
       <c r="I40" s="16">
@@ -1588,12 +1586,12 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="29"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
       <c r="I41" s="16">
@@ -1602,12 +1600,12 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="31"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="44"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17">
@@ -1616,12 +1614,12 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="72"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="36"/>
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="20">
@@ -1630,49 +1628,49 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="72"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
       <c r="I44" s="20"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="71"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="72"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="36"/>
       <c r="I45" s="20">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="71"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="72"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
       <c r="I46" s="20"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="73" t="s">
+      <c r="C47" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="67">
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="25">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="68"/>
-      <c r="I47" s="69"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -1681,6 +1679,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1697,43 +1732,6 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change font for P/N and change right aligh for the description. closes #21
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -379,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -399,11 +406,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -413,6 +417,129 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,24 +547,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -461,136 +570,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1145,7 +1188,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,21 +1207,21 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -1192,7 +1235,7 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
@@ -1216,18 +1259,18 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="24" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="24" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="21" t="s">
         <v>31</v>
       </c>
       <c r="I10" s="7"/>
@@ -1244,18 +1287,18 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
       <c r="I12" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1266,40 +1309,40 @@
       <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="D14" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="78"/>
-      <c r="F14" s="77" t="s">
+      <c r="E14" s="40"/>
+      <c r="F14" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="78"/>
-      <c r="H14" s="79" t="s">
+      <c r="G14" s="40"/>
+      <c r="H14" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="78"/>
+      <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="32"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1309,97 +1352,97 @@
       <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="84"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="8"/>
       <c r="G17" s="10"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="44"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="46" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="48"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="67"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="69"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="72"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="72"/>
+      <c r="A24" s="51"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="72"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
@@ -1408,134 +1451,134 @@
       <c r="B26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="58" t="s">
+      <c r="C26" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="72"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="72"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="50"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="72"/>
+      <c r="A28" s="92"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="72"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="72"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="72"/>
+      <c r="A31" s="92"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="75"/>
+      <c r="A32" s="93"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="53"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="48"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="49" t="s">
+      <c r="B35" s="55"/>
+      <c r="C35" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="55" t="s">
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="57" t="s">
+      <c r="H35" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="57" t="s">
+      <c r="I35" s="62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="42"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="75"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12">
@@ -1544,133 +1587,133 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16">
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15">
         <f t="shared" ref="I38:I43" si="0">H38*G38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16">
+      <c r="A40" s="25"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16">
+      <c r="A41" s="25"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17">
+      <c r="A42" s="27"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20">
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
-      <c r="I44" s="20"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="68"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="36"/>
-      <c r="I45" s="20">
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="68"/>
+      <c r="I45" s="17">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="I46" s="20"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="68"/>
+      <c r="I46" s="17"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="25">
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="63">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="26"/>
-      <c r="I47" s="27"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="65"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -1679,43 +1722,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1732,6 +1738,43 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Better format for TSR templates
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,13 +189,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -386,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -398,17 +391,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -417,6 +405,103 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -426,56 +511,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -485,6 +546,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -513,129 +592,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,7 +1196,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,79 +1215,79 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="7"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="7"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="7"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="21" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="21" t="s">
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="22" t="s">
         <v>31</v>
       </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1287,433 +1295,439 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="20" t="s">
+      <c r="B12" s="97"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="10"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="39" t="s">
+      <c r="E14" s="82"/>
+      <c r="F14" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41" t="s">
+      <c r="G14" s="82"/>
+      <c r="H14" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="40"/>
+      <c r="I14" s="82"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="26"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="85"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="26"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="85"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="96"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="10"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="93"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="28"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="87"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="22" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="24"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="50"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="76"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="76"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="76"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="50"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="76"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="76"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="76"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="50"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="76"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="93"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="53"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="79"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="52"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="54" t="s">
+      <c r="B35" s="54"/>
+      <c r="C35" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="60" t="s">
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="62" t="s">
+      <c r="H35" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="62" t="s">
+      <c r="I35" s="61" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
+      <c r="A36" s="55"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="72"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12">
+      <c r="A37" s="44"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26">
         <f>H37*G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15">
+      <c r="A38" s="35"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18">
         <f t="shared" ref="I38:I43" si="0">H38*G38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15">
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15">
+      <c r="A40" s="35"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15">
+      <c r="A41" s="35"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16">
+      <c r="A42" s="47"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17">
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="68"/>
-      <c r="I44" s="17"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="68"/>
-      <c r="I45" s="17">
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="27">
         <f>SUM(I37:I44)*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="68"/>
-      <c r="I46" s="17"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="27"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="63">
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="29">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="64"/>
-      <c r="I47" s="65"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -1722,6 +1736,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1738,43 +1789,6 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
COSMED logo updated - #45 fixed
</commit_message>
<xml_diff>
--- a/ConfigFiles/tsr_agreement.xlsx
+++ b/ConfigFiles/tsr_agreement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,6 +440,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -449,68 +512,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,15 +557,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
@@ -575,74 +593,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,13 +680,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>144145</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>28540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -694,15 +694,21 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1363345" cy="800100"/>
+          <a:off x="0" y="9560"/>
+          <a:ext cx="1363345" cy="780980"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -716,15 +722,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>504825</xdr:colOff>
+          <xdr:colOff>502920</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>83820</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -780,15 +786,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>504825</xdr:colOff>
+          <xdr:colOff>502920</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>83820</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -844,15 +850,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>504825</xdr:colOff>
+          <xdr:colOff>502920</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>83820</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1195,18 +1201,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1215,23 +1221,23 @@
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="3"/>
       <c r="C7" s="19"/>
@@ -1242,7 +1248,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
@@ -1255,7 +1261,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="3"/>
       <c r="C9" s="19"/>
@@ -1266,24 +1272,24 @@
       <c r="H9" s="19"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="22" t="s">
         <v>31</v>
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -1294,7 +1300,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>32</v>
       </c>
@@ -1309,7 +1315,7 @@
       <c r="H12" s="50"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1317,42 +1323,42 @@
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="51" t="s">
+      <c r="E14" s="83"/>
+      <c r="F14" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53" t="s">
+      <c r="G14" s="83"/>
+      <c r="H14" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="52"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="83"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="85"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="86"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="87"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="86"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -1360,233 +1366,233 @@
       <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="45"/>
+      <c r="E17" s="97"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="36"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="85"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="94"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="87"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="88"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="30" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="68"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="69"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="71"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="71"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="72"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="74"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="75"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="78"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="77"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="71"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="76"/>
+      <c r="I25" s="77"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="71"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="77"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="71"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="76"/>
+      <c r="I27" s="77"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="24"/>
       <c r="B28" s="24"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="71"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="77"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="24"/>
       <c r="B29" s="24"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="71"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="77"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="24"/>
       <c r="B30" s="24"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="71"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="77"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="24"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="71"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="77"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="74"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="80"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="32"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="53"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="79" t="s">
+      <c r="B35" s="55"/>
+      <c r="C35" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="85" t="s">
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="87" t="s">
+      <c r="H35" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="87" t="s">
+      <c r="I35" s="62" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="97"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="48"/>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="56"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="45"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="47"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26">
@@ -1594,13 +1600,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="78"/>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="37"/>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18">
@@ -1608,13 +1614,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="78"/>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="37"/>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="18">
@@ -1622,13 +1628,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="77"/>
-      <c r="B40" s="78"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="78"/>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="37"/>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" s="18">
@@ -1636,13 +1642,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="77"/>
-      <c r="B41" s="78"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="78"/>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="37"/>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" s="18">
@@ -1650,13 +1656,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="75"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="75"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="48"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="48"/>
       <c r="D42" s="50"/>
       <c r="E42" s="50"/>
-      <c r="F42" s="76"/>
+      <c r="F42" s="49"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17">
@@ -1664,13 +1670,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C43" s="91" t="s">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C43" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="92"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="93"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="27"/>
       <c r="H43" s="27"/>
       <c r="I43" s="27">
@@ -1678,24 +1684,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="91" t="s">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C44" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="93"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="27"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="91" t="s">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C45" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="93"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="27">
@@ -1703,39 +1709,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="91" t="s">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C46" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="92"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="93"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="27"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="94" t="s">
+    <row r="47" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C47" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="95"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="96"/>
-      <c r="G47" s="88">
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="30">
         <f>SUM(I37:I44)+I45-I46</f>
         <v>0</v>
       </c>
-      <c r="H47" s="89"/>
-      <c r="I47" s="90"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H47" s="31"/>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F22:I32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A22:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:B36"/>
+    <mergeCell ref="C35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A41:B41"/>
@@ -1752,43 +1795,6 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:B36"/>
-    <mergeCell ref="C35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F22:I32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D15:E16"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1804,15 +1810,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:colOff>502920</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>83820</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>106680</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1826,15 +1832,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:colOff>502920</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>83820</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>106680</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -1848,15 +1854,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>7</xdr:col>
-                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:colOff>502920</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>83820</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>106680</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>